<commit_message>
Some changes to all the files
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Finn\OneDrive - University of Bristol\Documents\ATMD\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/qt19495_bristol_ac_uk/Documents/year 4/ATMD/coursework/ATMD_coursework/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F30AB98-D947-46C0-86BE-CD8A678F43B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{3F30AB98-D947-46C0-86BE-CD8A678F43B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76E516B9-5A51-4CF8-ABFE-60DF38D9438C}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{7881286F-9FE5-4E29-AB54-BAE31099D7FA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7881286F-9FE5-4E29-AB54-BAE31099D7FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Engine Data" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <t>Engine</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>ISP</t>
+  </si>
+  <si>
+    <t>Fuel Price</t>
   </si>
 </sst>
 </file>
@@ -231,6 +234,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -530,27 +537,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB017142-5A60-4F53-9909-283A091E7519}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.31640625" customWidth="1"/>
+    <col min="2" max="2" width="16.26953125" customWidth="1"/>
     <col min="4" max="4" width="9.26953125" customWidth="1"/>
     <col min="5" max="5" width="12.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.81640625" customWidth="1"/>
-    <col min="7" max="7" width="8.58984375" customWidth="1"/>
-    <col min="8" max="8" width="9.31640625" customWidth="1"/>
+    <col min="7" max="7" width="8.54296875" customWidth="1"/>
+    <col min="8" max="8" width="9.26953125" customWidth="1"/>
     <col min="9" max="9" width="10.26953125" customWidth="1"/>
-    <col min="10" max="10" width="8.76953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7265625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -578,8 +585,11 @@
       <c r="I1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -607,8 +617,11 @@
       <c r="I2">
         <v>9750</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J2">
+        <v>75.12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -636,8 +649,11 @@
       <c r="I3">
         <v>5480</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J3">
+        <v>75.12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -665,8 +681,11 @@
       <c r="I4">
         <v>1250</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J4">
+        <v>75.12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -694,8 +713,11 @@
       <c r="I5">
         <v>8391</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J5">
+        <v>93.87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -723,8 +745,11 @@
       <c r="I6">
         <v>1610</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J6">
+        <v>93.87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -752,8 +777,11 @@
       <c r="I7">
         <v>1027</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J7">
+        <v>93.87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -781,8 +809,11 @@
       <c r="I8">
         <v>1300</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -810,8 +841,11 @@
       <c r="I9">
         <v>712.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -839,8 +873,11 @@
       <c r="I10">
         <v>826</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -868,8 +905,11 @@
       <c r="I11">
         <v>6600</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -897,8 +937,11 @@
       <c r="I12">
         <v>1250</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J12">
+        <v>75.12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -926,8 +969,11 @@
       <c r="I13">
         <v>826</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -955,8 +1001,11 @@
       <c r="I14">
         <v>712.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -982,10 +1031,13 @@
         <v>2.4300000000000002</v>
       </c>
       <c r="I15">
-        <v>6.5970000000000004</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.75">
+        <v>6597</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1013,8 +1065,11 @@
       <c r="I16">
         <v>3177</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1042,8 +1097,11 @@
       <c r="I17">
         <v>3450</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1071,8 +1129,11 @@
       <c r="I18">
         <v>1800</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1099,6 +1160,9 @@
       </c>
       <c r="I19">
         <v>811</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1111,15 +1175,15 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1127,12 +1191,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.5" x14ac:dyDescent="0.95">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1140,7 +1204,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1148,22 +1212,22 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -1388,13 +1452,39 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96BB6E09-EC4B-4582-922B-3CAF90EFAEB9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96BB6E09-EC4B-4582-922B-3CAF90EFAEB9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="028d60da-dcc2-4fe1-a4e0-fb3a7326d9df"/>
+    <ds:schemaRef ds:uri="a2f695cb-bd87-40de-8556-1bc463354fb8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0158D2AE-79CB-4269-B7A0-456F8D722B63}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0158D2AE-79CB-4269-B7A0-456F8D722B63}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F9D025E-6831-4532-8A82-D95821441953}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F9D025E-6831-4532-8A82-D95821441953}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a2f695cb-bd87-40de-8556-1bc463354fb8"/>
+    <ds:schemaRef ds:uri="028d60da-dcc2-4fe1-a4e0-fb3a7326d9df"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
1 - updating the code to Finn's version
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/qt19495_bristol_ac_uk/Documents/year 4/ATMD/coursework/ATMD_coursework/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Finn\OneDrive - University of Bristol\Documents\ATMD\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{3F30AB98-D947-46C0-86BE-CD8A678F43B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76E516B9-5A51-4CF8-ABFE-60DF38D9438C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F30AB98-D947-46C0-86BE-CD8A678F43B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7881286F-9FE5-4E29-AB54-BAE31099D7FA}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{7881286F-9FE5-4E29-AB54-BAE31099D7FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Engine Data" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>Engine</t>
   </si>
@@ -166,9 +166,6 @@
   </si>
   <si>
     <t>ISP</t>
-  </si>
-  <si>
-    <t>Fuel Price</t>
   </si>
 </sst>
 </file>
@@ -234,10 +231,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -537,27 +530,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB017142-5A60-4F53-9909-283A091E7519}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="16.26953125" customWidth="1"/>
+    <col min="2" max="2" width="16.31640625" customWidth="1"/>
     <col min="4" max="4" width="9.26953125" customWidth="1"/>
     <col min="5" max="5" width="12.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.81640625" customWidth="1"/>
-    <col min="7" max="7" width="8.54296875" customWidth="1"/>
-    <col min="8" max="8" width="9.26953125" customWidth="1"/>
+    <col min="7" max="7" width="8.58984375" customWidth="1"/>
+    <col min="8" max="8" width="9.31640625" customWidth="1"/>
     <col min="9" max="9" width="10.26953125" customWidth="1"/>
-    <col min="10" max="10" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.76953125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -585,11 +578,8 @@
       <c r="I1" t="s">
         <v>31</v>
       </c>
-      <c r="J1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -617,11 +607,8 @@
       <c r="I2">
         <v>9750</v>
       </c>
-      <c r="J2">
-        <v>75.12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -649,11 +636,8 @@
       <c r="I3">
         <v>5480</v>
       </c>
-      <c r="J3">
-        <v>75.12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -681,11 +665,8 @@
       <c r="I4">
         <v>1250</v>
       </c>
-      <c r="J4">
-        <v>75.12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -713,11 +694,8 @@
       <c r="I5">
         <v>8391</v>
       </c>
-      <c r="J5">
-        <v>93.87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -745,11 +723,8 @@
       <c r="I6">
         <v>1610</v>
       </c>
-      <c r="J6">
-        <v>93.87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -777,11 +752,8 @@
       <c r="I7">
         <v>1027</v>
       </c>
-      <c r="J7">
-        <v>93.87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -809,11 +781,8 @@
       <c r="I8">
         <v>1300</v>
       </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -841,11 +810,8 @@
       <c r="I9">
         <v>712.5</v>
       </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -873,11 +839,8 @@
       <c r="I10">
         <v>826</v>
       </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -905,11 +868,8 @@
       <c r="I11">
         <v>6600</v>
       </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -937,11 +897,8 @@
       <c r="I12">
         <v>1250</v>
       </c>
-      <c r="J12">
-        <v>75.12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -969,11 +926,8 @@
       <c r="I13">
         <v>826</v>
       </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1001,11 +955,8 @@
       <c r="I14">
         <v>712.5</v>
       </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1031,13 +982,10 @@
         <v>2.4300000000000002</v>
       </c>
       <c r="I15">
-        <v>6597</v>
-      </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+        <v>6.5970000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1065,11 +1013,8 @@
       <c r="I16">
         <v>3177</v>
       </c>
-      <c r="J16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1097,11 +1042,8 @@
       <c r="I17">
         <v>3450</v>
       </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1129,11 +1071,8 @@
       <c r="I18">
         <v>1800</v>
       </c>
-      <c r="J18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1160,9 +1099,6 @@
       </c>
       <c r="I19">
         <v>811</v>
-      </c>
-      <c r="J19">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1175,15 +1111,15 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="13.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1191,12 +1127,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="16.5" x14ac:dyDescent="0.95">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1204,7 +1140,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1212,22 +1148,22 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -1452,39 +1388,13 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96BB6E09-EC4B-4582-922B-3CAF90EFAEB9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="028d60da-dcc2-4fe1-a4e0-fb3a7326d9df"/>
-    <ds:schemaRef ds:uri="a2f695cb-bd87-40de-8556-1bc463354fb8"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35192351-CC2C-4F2C-805F-60A4D664E917}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0158D2AE-79CB-4269-B7A0-456F8D722B63}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4D4CB8-D21F-4A39-8F18-C386DDDC5CB5}"/>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F9D025E-6831-4532-8A82-D95821441953}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a2f695cb-bd87-40de-8556-1bc463354fb8"/>
-    <ds:schemaRef ds:uri="028d60da-dcc2-4fe1-a4e0-fb3a7326d9df"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3709222-F650-4B07-8B51-2A78B9842AA1}"/>
 </file>
</xml_diff>

<commit_message>
2 - Solving DeltaV problem
The changes are displayed with comments in the files
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Finn\OneDrive - University of Bristol\Documents\ATMD\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/qt19495_bristol_ac_uk/Documents/year 4/ATMD/coursework_git/ATMD_coursework/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F30AB98-D947-46C0-86BE-CD8A678F43B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{3F30AB98-D947-46C0-86BE-CD8A678F43B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C335833C-982C-4489-B77F-47882B3ADF52}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{7881286F-9FE5-4E29-AB54-BAE31099D7FA}"/>
+    <workbookView xWindow="1130" yWindow="1500" windowWidth="14400" windowHeight="7360" xr2:uid="{7881286F-9FE5-4E29-AB54-BAE31099D7FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Engine Data" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="60">
   <si>
     <t>Engine</t>
   </si>
@@ -166,13 +166,64 @@
   </si>
   <si>
     <t>ISP</t>
+  </si>
+  <si>
+    <t>11D58M</t>
+  </si>
+  <si>
+    <t>RD-0210</t>
+  </si>
+  <si>
+    <t>AESTUS</t>
+  </si>
+  <si>
+    <t>J-2</t>
+  </si>
+  <si>
+    <t>YF-75</t>
+  </si>
+  <si>
+    <t>LE-5B</t>
+  </si>
+  <si>
+    <t>HM7-B</t>
+  </si>
+  <si>
+    <t>VINCI</t>
+  </si>
+  <si>
+    <t>RL-10B</t>
+  </si>
+  <si>
+    <t>LO2/Kerosene</t>
+  </si>
+  <si>
+    <t>N2O4/UDMH</t>
+  </si>
+  <si>
+    <t>N2O4/MMH</t>
+  </si>
+  <si>
+    <t>LO2/LH2</t>
+  </si>
+  <si>
+    <t>LO2/LH3</t>
+  </si>
+  <si>
+    <t>LO2/LH4</t>
+  </si>
+  <si>
+    <t>LO2/LH5</t>
+  </si>
+  <si>
+    <t>LO2/LH6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +241,18 @@
       <color rgb="FF040C28"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="5"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -212,10 +275,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,27 +594,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB017142-5A60-4F53-9909-283A091E7519}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.31640625" customWidth="1"/>
+    <col min="2" max="2" width="16.26953125" customWidth="1"/>
     <col min="4" max="4" width="9.26953125" customWidth="1"/>
     <col min="5" max="5" width="12.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.81640625" customWidth="1"/>
-    <col min="7" max="7" width="8.58984375" customWidth="1"/>
-    <col min="8" max="8" width="9.31640625" customWidth="1"/>
+    <col min="7" max="7" width="8.54296875" customWidth="1"/>
+    <col min="8" max="8" width="9.26953125" customWidth="1"/>
     <col min="9" max="9" width="10.26953125" customWidth="1"/>
-    <col min="10" max="10" width="8.76953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7265625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -579,7 +643,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -608,7 +672,7 @@
         <v>9750</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -637,7 +701,7 @@
         <v>5480</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -666,7 +730,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -695,7 +759,7 @@
         <v>8391</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -724,7 +788,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -753,7 +817,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -782,7 +846,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -811,7 +875,7 @@
         <v>712.5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -840,7 +904,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -869,7 +933,7 @@
         <v>6600</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -898,7 +962,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -927,7 +991,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -956,7 +1020,7 @@
         <v>712.5</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -985,7 +1049,7 @@
         <v>6.5970000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1014,7 +1078,7 @@
         <v>3177</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1043,7 +1107,7 @@
         <v>3450</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1072,7 +1136,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1101,8 +1165,271 @@
         <v>811</v>
       </c>
     </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20">
+        <v>79.5</v>
+      </c>
+      <c r="D20">
+        <v>353</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21">
+        <v>582</v>
+      </c>
+      <c r="D21">
+        <v>327</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22">
+        <v>582</v>
+      </c>
+      <c r="D22">
+        <v>325</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23">
+        <v>890</v>
+      </c>
+      <c r="D23">
+        <v>426</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24">
+        <v>79</v>
+      </c>
+      <c r="D24">
+        <v>440</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25">
+        <v>137</v>
+      </c>
+      <c r="D25">
+        <v>447</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>447</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>465</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>462</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>301</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1114,12 +1441,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1127,12 +1454,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.5" x14ac:dyDescent="0.95">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1140,7 +1467,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1148,22 +1475,22 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -1177,6 +1504,26 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a2f695cb-bd87-40de-8556-1bc463354fb8" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="028d60da-dcc2-4fe1-a4e0-fb3a7326d9df">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000D8140269C0E644F937BE1F1A9118B0C" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e051d1041117c4587b6a35ab60cbb63d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="028d60da-dcc2-4fe1-a4e0-fb3a7326d9df" xmlns:ns3="a2f695cb-bd87-40de-8556-1bc463354fb8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e979a8630860ab35469e9aebd1bf7862" ns2:_="" ns3:_="">
     <xsd:import namespace="028d60da-dcc2-4fe1-a4e0-fb3a7326d9df"/>
@@ -1359,26 +1706,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a2f695cb-bd87-40de-8556-1bc463354fb8" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="028d60da-dcc2-4fe1-a4e0-fb3a7326d9df">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DE0BCBB-263C-4B84-8690-B936B5510BA5}">
   <ds:schemaRefs>
@@ -1388,13 +1715,39 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35192351-CC2C-4F2C-805F-60A4D664E917}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3709222-F650-4B07-8B51-2A78B9842AA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a2f695cb-bd87-40de-8556-1bc463354fb8"/>
+    <ds:schemaRef ds:uri="028d60da-dcc2-4fe1-a4e0-fb3a7326d9df"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4D4CB8-D21F-4A39-8F18-C386DDDC5CB5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4D4CB8-D21F-4A39-8F18-C386DDDC5CB5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3709222-F650-4B07-8B51-2A78B9842AA1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35192351-CC2C-4F2C-805F-60A4D664E917}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="028d60da-dcc2-4fe1-a4e0-fb3a7326d9df"/>
+    <ds:schemaRef ds:uri="a2f695cb-bd87-40de-8556-1bc463354fb8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>